<commit_message>
Parent tree mapping updated 29/04/25
</commit_message>
<xml_diff>
--- a/data/Parent_Child_ID_Mapping.xlsx
+++ b/data/Parent_Child_ID_Mapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IDEATEC\VICTUS Machinery energy analysis\Parent child HIerarchy analysis for MVP-1 Using Python -Jan-25 data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dash Plotly\Parent_Child_Energy_Reconciliation-3 - Copy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5A2AF0-071D-4DB2-8228-A1FE3CE0E5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368F20C3-3FAC-4D1C-9B1C-EB37EC95ED10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7E387629-B6E3-4A75-935D-655B448141FA}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$94</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$99</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -78,7 +78,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -101,15 +101,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,10 +456,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{654095A2-EE73-4DC5-93FA-624660E0D573}">
-  <dimension ref="A1:B94"/>
+  <dimension ref="A1:B99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M104" sqref="M104"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -914,7 +927,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="B58" s="1">
         <v>74</v>
@@ -922,23 +935,23 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="B59" s="1">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
-        <v>123</v>
+        <v>76</v>
       </c>
       <c r="B60" s="1">
-        <v>201</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
-        <v>202</v>
+        <v>123</v>
       </c>
       <c r="B61" s="1">
         <v>201</v>
@@ -946,55 +959,55 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
+        <v>202</v>
+      </c>
+      <c r="B62" s="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
+        <v>131</v>
+      </c>
+      <c r="B63" s="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
         <v>221</v>
       </c>
-      <c r="B62" s="1">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="2">
-        <v>127</v>
-      </c>
-      <c r="B63" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="2">
-        <v>93</v>
-      </c>
-      <c r="B64" s="2">
-        <v>19</v>
+      <c r="B64" s="1">
+        <v>201</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c r="B65" s="2">
         <v>19</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="1">
-        <v>57</v>
-      </c>
-      <c r="B66" s="1">
-        <v>113</v>
+      <c r="A66" s="2">
+        <v>93</v>
+      </c>
+      <c r="B66" s="2">
+        <v>19</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="1">
-        <v>56</v>
-      </c>
-      <c r="B67" s="1">
-        <v>113</v>
+      <c r="A67" s="2">
+        <v>95</v>
+      </c>
+      <c r="B67" s="2">
+        <v>19</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B68" s="1">
         <v>113</v>
@@ -1002,7 +1015,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="B69" s="1">
         <v>113</v>
@@ -1010,7 +1023,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B70" s="1">
         <v>113</v>
@@ -1018,7 +1031,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B71" s="1">
         <v>113</v>
@@ -1026,7 +1039,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B72" s="1">
         <v>113</v>
@@ -1034,7 +1047,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B73" s="1">
         <v>113</v>
@@ -1042,7 +1055,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B74" s="1">
         <v>113</v>
@@ -1050,7 +1063,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B75" s="1">
         <v>113</v>
@@ -1058,7 +1071,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B76" s="1">
         <v>113</v>
@@ -1066,7 +1079,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B77" s="1">
         <v>113</v>
@@ -1074,23 +1087,23 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
-        <v>124</v>
+        <v>53</v>
       </c>
       <c r="B78" s="1">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
-        <v>210</v>
+        <v>65</v>
       </c>
       <c r="B79" s="1">
-        <v>211</v>
+        <v>113</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B80" s="1">
         <v>113</v>
@@ -1098,71 +1111,71 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
-        <v>118</v>
+        <v>64</v>
       </c>
       <c r="B81" s="1">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="B82" s="1">
-        <v>102</v>
+        <v>119</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
-        <v>102</v>
+        <v>210</v>
       </c>
       <c r="B83" s="1">
-        <v>101</v>
+        <v>211</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
-        <v>116</v>
+        <v>69</v>
       </c>
       <c r="B84" s="1">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
-        <v>60</v>
+        <v>118</v>
       </c>
       <c r="B85" s="1">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="B86" s="1">
-        <v>129</v>
+        <v>102</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="B87" s="1">
-        <v>129</v>
+        <v>101</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="B88" s="1">
-        <v>129</v>
+        <v>101</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="B89" s="1">
         <v>129</v>
@@ -1170,7 +1183,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
-        <v>125</v>
+        <v>61</v>
       </c>
       <c r="B90" s="1">
         <v>129</v>
@@ -1178,7 +1191,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B91" s="1">
         <v>129</v>
@@ -1186,7 +1199,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="B92" s="1">
         <v>129</v>
@@ -1194,22 +1207,62 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
-        <v>101</v>
+        <v>36</v>
       </c>
       <c r="B93" s="1">
-        <v>122</v>
+        <v>129</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
+        <v>125</v>
+      </c>
+      <c r="B94" s="1">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" s="1">
+        <v>58</v>
+      </c>
+      <c r="B95" s="1">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" s="1">
+        <v>59</v>
+      </c>
+      <c r="B96" s="1">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="1">
+        <v>101</v>
+      </c>
+      <c r="B97" s="1">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="1">
         <v>223</v>
       </c>
-      <c r="B94" s="1">
+      <c r="B98" s="1">
         <v>223</v>
       </c>
     </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="4">
+        <v>7</v>
+      </c>
+      <c r="B99" s="4">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B94" xr:uid="{654095A2-EE73-4DC5-93FA-624660E0D573}"/>
+  <autoFilter ref="A1:B99" xr:uid="{654095A2-EE73-4DC5-93FA-624660E0D573}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>